<commit_message>
NY and NJ completed
</commit_message>
<xml_diff>
--- a/data_collection/errors_1617.xlsx
+++ b/data_collection/errors_1617.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/Mines/S3/TR/econometrics/data_collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1D9BB7-3C47-9345-B461-291DE4AE8C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5450D9-2248-7149-AC32-430EF7876C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B9384D9D-633D-7741-83A9-0F3C7C0EABE7}"/>
   </bookViews>
@@ -507,6 +507,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,87 +595,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59049483-83BC-394D-BD70-81543C39E257}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="187" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,782 +930,782 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2">
+      <c r="B1" s="29">
         <v>2016</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2">
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="29">
         <v>2017</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="21">
-        <v>-1</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="18">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="18">
         <v>14</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <v>-12</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="21">
+      <c r="D7" s="20"/>
+      <c r="E7" s="18">
         <v>9</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="19">
         <v>-7</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23">
-        <v>-1</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20">
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22">
-        <v>1</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22">
-        <v>1</v>
-      </c>
-      <c r="G9" s="23"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="26">
         <v>3</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="27">
         <v>-3</v>
       </c>
-      <c r="D12" s="31">
-        <v>1</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30">
-        <v>1</v>
-      </c>
-      <c r="G12" s="31"/>
+      <c r="D12" s="28">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27">
+        <v>1</v>
+      </c>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="25">
-        <v>1</v>
-      </c>
-      <c r="C13" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D13" s="23">
+      <c r="B13" s="22">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="20">
         <v>-2</v>
       </c>
-      <c r="E13" s="25">
-        <v>1</v>
-      </c>
-      <c r="F13" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="23">
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="20">
         <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="26">
         <v>4</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="27">
         <v>-5</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="28">
         <v>-2</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31">
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28">
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="25">
-        <v>1</v>
-      </c>
-      <c r="C17" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D17" s="23">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="25">
-        <v>1</v>
-      </c>
-      <c r="F17" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G17" s="23">
+      <c r="B17" s="22">
+        <v>1</v>
+      </c>
+      <c r="C17" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="22">
+        <v>1</v>
+      </c>
+      <c r="F17" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="20">
         <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="25">
-        <v>1</v>
-      </c>
-      <c r="C18" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="25">
-        <v>1</v>
-      </c>
-      <c r="F18" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G18" s="23"/>
+      <c r="B18" s="22">
+        <v>1</v>
+      </c>
+      <c r="C18" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="22">
+        <v>1</v>
+      </c>
+      <c r="F18" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="25">
-        <v>1</v>
-      </c>
-      <c r="C19" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D19" s="23">
-        <v>-1</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23">
+      <c r="B19" s="22">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D19" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20">
         <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="25">
-        <v>-1</v>
-      </c>
-      <c r="C20" s="26">
-        <v>1</v>
-      </c>
-      <c r="D20" s="23">
+      <c r="B20" s="22">
+        <v>-1</v>
+      </c>
+      <c r="C20" s="23">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20">
         <v>-2</v>
       </c>
-      <c r="E20" s="25">
-        <v>-1</v>
-      </c>
-      <c r="F20" s="26">
-        <v>1</v>
-      </c>
-      <c r="G20" s="23">
+      <c r="E20" s="22">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="23">
+        <v>1</v>
+      </c>
+      <c r="G20" s="20">
         <v>-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="22">
         <v>2</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="23">
         <v>-2</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="25">
-        <v>1</v>
-      </c>
-      <c r="F23" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G23" s="23"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="22">
+        <v>1</v>
+      </c>
+      <c r="F23" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="15"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="15"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22">
-        <v>-1</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19">
+        <v>-1</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19">
+        <v>-1</v>
+      </c>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31">
-        <v>-1</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28">
+        <v>-1</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="25">
-        <v>1</v>
-      </c>
-      <c r="C32" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
+      <c r="B32" s="22">
+        <v>1</v>
+      </c>
+      <c r="C32" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B33" s="18">
         <v>4</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="19">
         <v>-5</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="21">
+      <c r="D33" s="20"/>
+      <c r="E33" s="18">
         <v>4</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="19">
         <v>-5</v>
       </c>
-      <c r="G33" s="23"/>
+      <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="21">
+      <c r="B35" s="18">
         <v>3</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="19">
         <v>-4</v>
       </c>
-      <c r="D35" s="23">
-        <v>-1</v>
-      </c>
-      <c r="E35" s="21">
-        <v>1</v>
-      </c>
-      <c r="F35" s="22">
+      <c r="D35" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E35" s="18">
+        <v>1</v>
+      </c>
+      <c r="F35" s="19">
         <v>-2</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="20">
         <v>-1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="25">
-        <v>-1</v>
-      </c>
-      <c r="C36" s="26">
-        <v>1</v>
-      </c>
-      <c r="D36" s="23">
+      <c r="B36" s="22">
+        <v>-1</v>
+      </c>
+      <c r="C36" s="23">
+        <v>1</v>
+      </c>
+      <c r="D36" s="20">
         <v>-3</v>
       </c>
-      <c r="E36" s="25">
-        <v>-1</v>
-      </c>
-      <c r="F36" s="26">
-        <v>1</v>
-      </c>
-      <c r="G36" s="23">
+      <c r="E36" s="22">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="23">
+        <v>1</v>
+      </c>
+      <c r="G36" s="20">
         <v>-3</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="15"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="25">
-        <v>1</v>
-      </c>
-      <c r="C38" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="25">
-        <v>1</v>
-      </c>
-      <c r="F38" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G38" s="27"/>
+      <c r="B38" s="22">
+        <v>1</v>
+      </c>
+      <c r="C38" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="22">
+        <v>1</v>
+      </c>
+      <c r="F38" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G38" s="24"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="15"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="15"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="15"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="15"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="15"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="12"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="15"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="12"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31">
-        <v>1</v>
-      </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="31"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28">
+        <v>1</v>
+      </c>
+      <c r="E45" s="26"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="29">
-        <v>1</v>
-      </c>
-      <c r="C46" s="30">
-        <v>-1</v>
-      </c>
-      <c r="D46" s="31">
-        <v>1</v>
-      </c>
-      <c r="E46" s="29">
-        <v>1</v>
-      </c>
-      <c r="F46" s="30"/>
-      <c r="G46" s="31">
+      <c r="B46" s="26">
+        <v>1</v>
+      </c>
+      <c r="C46" s="27">
+        <v>-1</v>
+      </c>
+      <c r="D46" s="28">
+        <v>1</v>
+      </c>
+      <c r="E46" s="26">
+        <v>1</v>
+      </c>
+      <c r="F46" s="27"/>
+      <c r="G46" s="28">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="15"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="12"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="25">
-        <v>1</v>
-      </c>
-      <c r="C48" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27"/>
+      <c r="B48" s="22">
+        <v>1</v>
+      </c>
+      <c r="C48" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D48" s="24"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="25">
-        <v>1</v>
-      </c>
-      <c r="C49" s="26">
-        <v>-1</v>
-      </c>
-      <c r="D49" s="27"/>
-      <c r="E49" s="25">
-        <v>1</v>
-      </c>
-      <c r="F49" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G49" s="27"/>
+      <c r="B49" s="22">
+        <v>1</v>
+      </c>
+      <c r="C49" s="23">
+        <v>-1</v>
+      </c>
+      <c r="D49" s="24"/>
+      <c r="E49" s="22">
+        <v>1</v>
+      </c>
+      <c r="F49" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="15"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="12"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="15"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="12"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B52" s="22">
         <v>2</v>
       </c>
-      <c r="C52" s="26">
+      <c r="C52" s="23">
         <v>-2</v>
       </c>
-      <c r="D52" s="27"/>
-      <c r="E52" s="25">
-        <v>1</v>
-      </c>
-      <c r="F52" s="26">
-        <v>-1</v>
-      </c>
-      <c r="G52" s="27"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="22">
+        <v>1</v>
+      </c>
+      <c r="F52" s="23">
+        <v>-1</v>
+      </c>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="19"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>